<commit_message>
- Anpassung Projektkosten - Anpassung Projektstatusbericht 3 - Hinzufügen Projektstatusbericht 4
</commit_message>
<xml_diff>
--- a/documents/projectmanagement/2_Definition/Projektkosten_PAMS_Verteilt.xlsx
+++ b/documents/projectmanagement/2_Definition/Projektkosten_PAMS_Verteilt.xlsx
@@ -138,9 +138,6 @@
     <t>4h, durch Techniker</t>
   </si>
   <si>
-    <t xml:space="preserve">25h, Logik, Ausgabe, Eingabe, Datenbankzugriff, Login(Verschlüsselung), </t>
-  </si>
-  <si>
     <t>8h, DB-Design, Erstellung</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>32h, Machbarkeit, Umfeld, Risiko, Statusberichte, Kommunikationsrichtlinien, Dokumentationsrichtlinien</t>
+  </si>
+  <si>
+    <t>25h, Logik, Ausgabe, Eingabe, Datenbankzugriff, Login(Verschlüsselung), Frontend</t>
   </si>
 </sst>
 </file>
@@ -262,6 +262,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -270,15 +279,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -592,8 +592,8 @@
   </sheetPr>
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,18 +604,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -674,11 +674,11 @@
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -731,14 +731,14 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -749,18 +749,18 @@
         <v>681.6</v>
       </c>
       <c r="C15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="13">
+        <v>4368</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="16">
-        <v>4368</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -775,14 +775,14 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="13">
         <v>3417.6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>